<commit_message>
chages  on weekly report
</commit_message>
<xml_diff>
--- a/data/ncis-sprint-burndowns.xlsx
+++ b/data/ncis-sprint-burndowns.xlsx
@@ -3,19 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901685F5-343D-4648-9169-3F24052836B8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47FF3BF-63C1-4D1C-87A9-145DEA045730}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="DEV Status" sheetId="7" r:id="rId1"/>
-    <sheet name="QA Status" sheetId="10" r:id="rId2"/>
-    <sheet name="Data" sheetId="5" r:id="rId3"/>
-    <sheet name="SP" sheetId="8" r:id="rId4"/>
-    <sheet name="Sprints" sheetId="9" r:id="rId5"/>
+    <sheet name="EPIC Status" sheetId="11" r:id="rId1"/>
+    <sheet name="DEV Status" sheetId="7" r:id="rId2"/>
+    <sheet name="QA Status" sheetId="10" r:id="rId3"/>
+    <sheet name="Data" sheetId="5" r:id="rId4"/>
+    <sheet name="SP" sheetId="8" r:id="rId5"/>
+    <sheet name="Sprints" sheetId="9" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Data!$B$1:$L$60</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Data!$B$1:$L$60</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="138">
   <si>
     <t>Backlog Sprint</t>
   </si>
@@ -448,6 +449,12 @@
   </si>
   <si>
     <t>READY</t>
+  </si>
+  <si>
+    <t>Backlog (Epics)</t>
+  </si>
+  <si>
+    <t>Ready (Epics)</t>
   </si>
 </sst>
 </file>
@@ -577,6 +584,628 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>EPIC</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Status</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'EPIC Status'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Backlog (Epics)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'EPIC Status'!$A$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'EPIC Status'!$B$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>172</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7E7E-480D-91C9-22B4DF61EB2F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'EPIC Status'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ready (Epics)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'EPIC Status'!$A$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'EPIC Status'!$C$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7E7E-480D-91C9-22B4DF61EB2F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="800124863"/>
+        <c:axId val="902466623"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="800124863"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sprints</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="902466623"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="902466623"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Epics</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="800124863"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2167,7 +2796,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3850,8 +4479,48 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="352">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3862,7 +4531,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -3875,7 +4544,7 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
@@ -3892,7 +4561,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -3908,7 +4577,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -3952,20 +4621,20 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -3974,13 +4643,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="34925" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -3992,10 +4661,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3">
+    <cs:fillRef idx="1">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="3"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -4004,17 +4673,16 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="3"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
@@ -4118,8 +4786,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
@@ -4209,20 +4883,20 @@
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -4235,17 +4909,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -4277,7 +4940,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -4286,13 +4949,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -4346,8 +5010,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -4854,7 +5524,550 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="352">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AD0867F-E2B9-457A-8C41-93D78D3C80B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4895,7 +6108,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5200,10 +6413,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6340498-5864-4D42-B791-302F89C00490}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>18</v>
+      </c>
+      <c r="B2">
+        <v>172</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFF9B5FC-B68C-490C-BD95-2891DA1E6071}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
@@ -5629,7 +6881,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FC0E560-D797-42BC-BC56-CF69B6E909EF}">
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -6059,7 +7311,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B4C989A-0DB4-4957-8B7C-55617C9397A2}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T60"/>
@@ -10091,7 +11343,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6DA68DE-49B5-450C-B56C-8FE4562D72A6}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -10211,7 +11463,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B002830-2D91-48C2-9C27-20C71EEBA17A}">
   <dimension ref="A1:C20"/>
   <sheetViews>

</xml_diff>